<commit_message>
Added a loop for it to iterate every "Cedula" and make a request on the site for each one. Also added new lines to save the data into an xlsx file using pandas library.
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erick\PycharmProjects\webScrapingTSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671F48C7-4888-4A83-BDA8-FF5E955F36F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7CAFB1-36F6-4C27-9FFC-3FAFC6947C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{CE2F1C29-2C7B-42A6-ABF8-1A4466B1DF46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE2F1C29-2C7B-42A6-ABF8-1A4466B1DF46}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -36,27 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Cedula</t>
-  </si>
-  <si>
-    <t>Fecha Nacimiento</t>
-  </si>
-  <si>
-    <t>Padre</t>
-  </si>
-  <si>
-    <t>Madre</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Nombre Completo</t>
-  </si>
-  <si>
-    <t>Edad</t>
   </si>
 </sst>
 </file>
@@ -88,7 +70,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -96,29 +78,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA188BE-327C-49F7-BE5F-3C80DBBAB96B}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,49 +411,44 @@
     <col min="3" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>117100591</v>
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>118470695</v>
+        <v>117100592</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>117100593</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>117100594</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added import concurrent.futures to use threads to speed up the process. Also defined function "scrape_cedula"
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erick\PycharmProjects\webScrapingTSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7CAFB1-36F6-4C27-9FFC-3FAFC6947C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305EA780-77F2-4884-BF91-39F303F6E94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE2F1C29-2C7B-42A6-ABF8-1A4466B1DF46}"/>
   </bookViews>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA188BE-327C-49F7-BE5F-3C80DBBAB96B}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,12 +440,167 @@
       </c>
       <c r="D5" s="1"/>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>117100595</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>117100596</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>117100597</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>117100598</v>
+      </c>
+    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10">
+        <v>117100599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>117100600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>117100601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>117100602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>117100603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>117100604</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>117100605</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>117100606</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>117100607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>117100608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>117100609</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>117100610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>117100611</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>117100612</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>117100613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>117100614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>117100615</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>117100616</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>117100617</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>117100618</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>117100619</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>117100620</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>117100621</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>117100622</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>117100623</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>117100624</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>117100625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>117100626</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added access to the more details page, while using the same request session.
</commit_message>
<xml_diff>
--- a/cedulas.xlsx
+++ b/cedulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erick\PycharmProjects\webScrapingTSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305EA780-77F2-4884-BF91-39F303F6E94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667D7A7B-A957-4C18-98C0-777DFE769987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE2F1C29-2C7B-42A6-ABF8-1A4466B1DF46}"/>
   </bookViews>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA188BE-327C-49F7-BE5F-3C80DBBAB96B}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +602,11 @@
         <v>117100626</v>
       </c>
     </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>117050399</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>